<commit_message>
Add manipulations and conversions test cases to Final-Project-Test-Cases.xlsx
</commit_message>
<xml_diff>
--- a/V2/manipulations/manipulation-test-cases.xlsx
+++ b/V2/manipulations/manipulation-test-cases.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\Desktop\Manipulation V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/adsmith6_myseneca_ca/Documents/CPR101/finalProject/project/git/CPR101group3/V2/manipulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFBFB89-9262-433A-9E42-035B7278758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{2DFBFB89-9262-433A-9E42-035B7278758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048754B9-135D-4523-9A13-D3C23541C242}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to be deleted" sheetId="2" r:id="rId1"/>
-    <sheet name="-the-name-of-your- module" sheetId="3" r:id="rId2"/>
+    <sheet name="manipulations" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'example to be deleted'!#REF!</definedName>
@@ -1832,6 +1832,15 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1843,15 +1852,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2212,22 +2212,22 @@
       <c r="B1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="46" t="str">
+      <c r="C1" s="49" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="31"/>
       <c r="F2" s="18" t="s">
         <v>11</v>
@@ -2414,11 +2414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E121BC-7441-452D-BF7D-1BC2B8D0CBF7}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2439,23 +2439,23 @@
       <c r="B1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="46" t="str">
+      <c r="C1" s="49" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As Manipulation_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2605,13 +2605,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="20" t="s">
         <v>11</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="C13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="44" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="3"/>
@@ -2679,7 +2679,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="45" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="29" t="s">
@@ -2688,7 +2688,7 @@
       <c r="C14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="44" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="3"/>
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="45" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="29" t="s">
@@ -2706,7 +2706,7 @@
       <c r="C15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="44" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="3"/>
@@ -2739,7 +2739,7 @@
       <c r="B17" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="46" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="24" t="s">
@@ -2754,13 +2754,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="20" t="s">
         <v>11</v>
       </c>

</xml_diff>